<commit_message>
uploaded created files from 6 HW
</commit_message>
<xml_diff>
--- a/HW_6/output_files/Katser_M_less_6_Task_5.xlsx
+++ b/HW_6/output_files/Katser_M_less_6_Task_5.xlsx
@@ -536,32 +536,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+375(44)4763516</t>
+          <t>+375(29)8243623</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>+375(44)9308068</t>
+          <t>+375(44)9623454</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+375(33)9046179</t>
+          <t>+375(33)8714775</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+375(29)1609948</t>
+          <t>+375(44)1317654</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>+375(33)8768613</t>
+          <t>+375(44)1635345</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+375(33)5275900</t>
+          <t>+375(44)8421539</t>
         </is>
       </c>
     </row>

</xml_diff>